<commit_message>
Excel read/write feature integrated to price check
</commit_message>
<xml_diff>
--- a/item_prices.xlsx
+++ b/item_prices.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Item Name</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>speaker</t>
-  </si>
-  <si>
-    <t>kitchen mixer</t>
   </si>
 </sst>
 </file>
@@ -318,11 +315,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>